<commit_message>
succes task Arif_12(Prio2k) filename 90.0792
</commit_message>
<xml_diff>
--- a/Arif_12(Prio2k)/Arif_12(Prio2k).xlsx
+++ b/Arif_12(Prio2k)/Arif_12(Prio2k).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif_12(Prio2k)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68935469-1705-4976-BDCA-3430D9FB9BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B95D3F-701D-42CC-B596-7B7B1119E81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,9 +240,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +297,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Eurostile"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,7 +380,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -387,10 +417,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1">
@@ -408,13 +438,34 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -909,7 +960,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1013,81 +1064,97 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="9">
+    <row r="5" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A5" s="17">
+        <v>433</v>
+      </c>
+      <c r="B5" s="21">
+        <v>45173</v>
+      </c>
+      <c r="C5" s="18">
         <v>90.078699999999998</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="9">
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" s="30" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A6" s="25">
+        <v>119</v>
+      </c>
+      <c r="B6" s="26">
+        <v>45174</v>
+      </c>
+      <c r="C6" s="27">
         <v>90.078999999999994</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A7" s="13"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="9">
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+    </row>
+    <row r="7" spans="1:9" s="30" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A7" s="25">
+        <v>8</v>
+      </c>
+      <c r="B7" s="26">
+        <v>45174</v>
+      </c>
+      <c r="C7" s="27">
         <v>90.079099999999997</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="9">
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+    </row>
+    <row r="8" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A8" s="17">
+        <v>94</v>
+      </c>
+      <c r="B8" s="21">
+        <v>45174</v>
+      </c>
+      <c r="C8" s="18">
         <v>90.0792</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
       <c r="A9" s="13"/>
@@ -1269,7 +1336,7 @@
       <c r="D18" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="16" t="s">
         <v>43</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -1288,7 +1355,7 @@
       <c r="D19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="16" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="10" t="s">
@@ -1298,43 +1365,51 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="9">
+    <row r="20" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A20" s="17">
+        <v>23</v>
+      </c>
+      <c r="B20" s="21">
+        <v>45173</v>
+      </c>
+      <c r="C20" s="18">
         <v>90.083399999999997</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="9">
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A21" s="17">
+        <v>21</v>
+      </c>
+      <c r="B21" s="21">
+        <v>45173</v>
+      </c>
+      <c r="C21" s="18">
         <v>90.083500000000001</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9">
       <c r="C22" s="5"/>
@@ -1351,6 +1426,13 @@
     <hyperlink ref="E3" r:id="rId2" xr:uid="{2A827E9D-34B3-4624-99B3-3F0CD8C21271}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{B8CBECEF-8710-437B-B52F-E0126D31C0D2}"/>
     <hyperlink ref="E5" r:id="rId4" location="pos" xr:uid="{D89C4DE8-BE3F-4A44-93F4-88173DC141E8}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{91DF895D-1862-4101-BE83-6CFE5791E13D}"/>
+    <hyperlink ref="E19" r:id="rId6" xr:uid="{AFD56E93-AFF6-48C0-868C-4F0477C3E7A6}"/>
+    <hyperlink ref="E20" r:id="rId7" xr:uid="{0B6F44F3-D838-4158-9E0A-D643CE9F90C2}"/>
+    <hyperlink ref="E21" r:id="rId8" xr:uid="{0C1BEB9C-14A1-4571-AA98-C47D7BFA68C6}"/>
+    <hyperlink ref="E18" r:id="rId9" xr:uid="{C8AE74BD-686E-4FA6-9300-BF7C6FCE4B71}"/>
+    <hyperlink ref="E7" r:id="rId10" xr:uid="{846B62B6-4484-4060-8F35-C863E126CF36}"/>
+    <hyperlink ref="E8" r:id="rId11" xr:uid="{09613F1A-C181-4D3D-9965-4CA3A816404A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
succes task Arif_12(Prio2k) filename 90.0802
</commit_message>
<xml_diff>
--- a/Arif_12(Prio2k)/Arif_12(Prio2k).xlsx
+++ b/Arif_12(Prio2k)/Arif_12(Prio2k).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif_12(Prio2k)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B95D3F-701D-42CC-B596-7B7B1119E81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F165030A-EBCC-4FF0-B094-27701EA380F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,12 +338,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +374,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -402,30 +396,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -447,25 +423,22 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -959,16 +932,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="12"/>
-    <col min="2" max="2" width="19" style="14" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="9"/>
+    <col min="2" max="2" width="19" style="10" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="59.28515625" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" customWidth="1"/>
     <col min="5" max="5" width="95.5703125" customWidth="1"/>
     <col min="6" max="6" width="85.140625" customWidth="1"/>
     <col min="9" max="9" width="64.5703125" customWidth="1"/>
@@ -997,419 +970,459 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A2" s="17">
+    <row r="2" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A2" s="11">
         <v>78</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="15">
         <v>45173</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="12">
         <v>90.074799999999996</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A3" s="17">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A3" s="11">
         <v>6</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="15">
         <v>45173</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="12">
         <v>90.077299999999994</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="17">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A4" s="11">
         <v>204</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="15">
         <v>45173</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="12">
         <v>90.078299999999999</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A5" s="17">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A5" s="11">
         <v>433</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="15">
         <v>45173</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="12">
         <v>90.078699999999998</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" s="30" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A6" s="25">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A6" s="11">
         <v>119</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="15">
         <v>45174</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="12">
         <v>90.078999999999994</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-    </row>
-    <row r="7" spans="1:9" s="30" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A7" s="25">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A7" s="11">
         <v>8</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="15">
         <v>45174</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="12">
         <v>90.079099999999997</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-    </row>
-    <row r="8" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A8" s="17">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A8" s="11">
         <v>94</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="15">
         <v>45174</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="12">
         <v>90.0792</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-    </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="9">
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A9" s="11">
+        <v>100</v>
+      </c>
+      <c r="B9" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C9" s="12">
         <v>90.079300000000003</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="9">
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A10" s="11">
+        <v>62</v>
+      </c>
+      <c r="B10" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C10" s="12">
         <v>90.079400000000007</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A11" s="13"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="9">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A11" s="11">
+        <v>22</v>
+      </c>
+      <c r="B11" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C11" s="12">
         <v>90.079499999999996</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="9">
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A12" s="11">
+        <v>14</v>
+      </c>
+      <c r="B12" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C12" s="12">
         <v>90.079599999999999</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="9">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A13" s="11">
+        <v>180</v>
+      </c>
+      <c r="B13" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C13" s="12">
         <v>90.079700000000003</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="9">
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A14" s="11">
+        <v>137</v>
+      </c>
+      <c r="B14" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C14" s="12">
         <v>90.079800000000006</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="9">
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A15" s="11">
+        <v>954</v>
+      </c>
+      <c r="B15" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C15" s="12">
         <v>90.079899999999995</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="9">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A16" s="11">
+        <v>198</v>
+      </c>
+      <c r="B16" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C16" s="12">
         <v>90.08</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="9">
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A17" s="11">
+        <v>26</v>
+      </c>
+      <c r="B17" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C17" s="12">
         <v>90.080100000000002</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="9">
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A18" s="11">
+        <v>398</v>
+      </c>
+      <c r="B18" s="15">
+        <v>45174</v>
+      </c>
+      <c r="C18" s="12">
         <v>90.080200000000005</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-    </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="9">
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" s="23" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20">
         <v>90.082999999999998</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A20" s="17">
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+    </row>
+    <row r="20" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A20" s="11">
         <v>23</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="15">
         <v>45173</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="12">
         <v>90.083399999999997</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-    </row>
-    <row r="21" spans="1:9" s="20" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A21" s="17">
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" s="14" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A21" s="11">
         <v>21</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="15">
         <v>45173</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="12">
         <v>90.083500000000001</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9">
       <c r="C22" s="5"/>
@@ -1433,6 +1446,15 @@
     <hyperlink ref="E18" r:id="rId9" xr:uid="{C8AE74BD-686E-4FA6-9300-BF7C6FCE4B71}"/>
     <hyperlink ref="E7" r:id="rId10" xr:uid="{846B62B6-4484-4060-8F35-C863E126CF36}"/>
     <hyperlink ref="E8" r:id="rId11" xr:uid="{09613F1A-C181-4D3D-9965-4CA3A816404A}"/>
+    <hyperlink ref="E9" r:id="rId12" xr:uid="{BCF741D0-AE51-4A20-AFE3-6154B6DCF14B}"/>
+    <hyperlink ref="E10" r:id="rId13" xr:uid="{445C0076-5786-48EB-846B-ECF83815E60B}"/>
+    <hyperlink ref="E11" r:id="rId14" xr:uid="{D4BD62D8-10AA-4F62-9BC5-D346F85F93B2}"/>
+    <hyperlink ref="E12" r:id="rId15" xr:uid="{35A01872-43AB-42F8-A122-D302EDACA9FA}"/>
+    <hyperlink ref="E13" r:id="rId16" xr:uid="{BF7B1225-C9CA-45D6-908C-7C87DF551E9A}"/>
+    <hyperlink ref="E14" r:id="rId17" xr:uid="{F5282A9E-EFCC-491D-877F-08A9ABD6DCE2}"/>
+    <hyperlink ref="E15" r:id="rId18" xr:uid="{60200A42-8BCE-4274-96C1-C65F2C948D17}"/>
+    <hyperlink ref="E16" r:id="rId19" xr:uid="{461DEFF8-1451-4CC1-BD34-F2B3A077DC98}"/>
+    <hyperlink ref="E17" r:id="rId20" xr:uid="{0F4CC2BA-4FD7-4405-8AA7-00F50705C79E}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>